<commit_message>
add content algo and content notebook
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Metis_Bootcamp\Business_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B77F93A-B7C5-4C8A-9C50-0EBDD1A4A4CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1468AD55-E669-4642-9FD2-0C5EBEB0FCEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A2134E5-29DB-41F3-83C9-30FC61C83E4B}"/>
+    <workbookView xWindow="3636" yWindow="1740" windowWidth="17280" windowHeight="10056" xr2:uid="{5A2134E5-29DB-41F3-83C9-30FC61C83E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Algorithms</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>SVD++</t>
+  </si>
+  <si>
+    <t>Content</t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3D42F8-DAEB-47CD-95E3-2501C98C4719}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,6 +498,17 @@
         <v>1.1415</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1.0158</v>
+      </c>
+      <c r="C7">
+        <v>0.78820000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>